<commit_message>
Data seed qualification and profession
</commit_message>
<xml_diff>
--- a/Documents/AllPanchayathWithIDs.xlsx
+++ b/Documents/AllPanchayathWithIDs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="UAEState" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,8 @@
     <sheet name="District" sheetId="3" r:id="rId3"/>
     <sheet name="Mandalam" sheetId="4" r:id="rId4"/>
     <sheet name="Panchayath" sheetId="5" r:id="rId5"/>
+    <sheet name="Professions" sheetId="6" r:id="rId6"/>
+    <sheet name="Qualifications" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7951" uniqueCount="2334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8202" uniqueCount="2582">
   <si>
     <t>Id</t>
   </si>
@@ -7228,12 +7230,756 @@
       <t>()),</t>
     </r>
   </si>
+  <si>
+    <t>ACCOUNTANT</t>
+  </si>
+  <si>
+    <t>ACTOR</t>
+  </si>
+  <si>
+    <t>ACTRESS</t>
+  </si>
+  <si>
+    <t>AIR TRAFFIC CONTROLLER</t>
+  </si>
+  <si>
+    <t>ARCHITECT</t>
+  </si>
+  <si>
+    <t>ARTIST</t>
+  </si>
+  <si>
+    <t>ATTORNEY</t>
+  </si>
+  <si>
+    <t>BANKER</t>
+  </si>
+  <si>
+    <t>BARTENDER</t>
+  </si>
+  <si>
+    <t>BARBER</t>
+  </si>
+  <si>
+    <t>BOOKKEEPER</t>
+  </si>
+  <si>
+    <t>BUILDER</t>
+  </si>
+  <si>
+    <t>BUSINESSMAN</t>
+  </si>
+  <si>
+    <t>BUSINESSWOMAN</t>
+  </si>
+  <si>
+    <t>BUSINESSPERSON</t>
+  </si>
+  <si>
+    <t>BUTCHER</t>
+  </si>
+  <si>
+    <t>CARPENTER</t>
+  </si>
+  <si>
+    <t>CASHIER</t>
+  </si>
+  <si>
+    <t>CHEF</t>
+  </si>
+  <si>
+    <t>COACH</t>
+  </si>
+  <si>
+    <t>DENTAL HYGIENIST</t>
+  </si>
+  <si>
+    <t>DENTIST</t>
+  </si>
+  <si>
+    <t>DESIGNER</t>
+  </si>
+  <si>
+    <t>DEVELOPER</t>
+  </si>
+  <si>
+    <t>DIETICIAN</t>
+  </si>
+  <si>
+    <t>DOCTOR</t>
+  </si>
+  <si>
+    <t>ECONOMIST</t>
+  </si>
+  <si>
+    <t>EDITOR</t>
+  </si>
+  <si>
+    <t>ELECTRICIAN</t>
+  </si>
+  <si>
+    <t>ENGINEER</t>
+  </si>
+  <si>
+    <t>FARMER</t>
+  </si>
+  <si>
+    <t>FILMMAKER</t>
+  </si>
+  <si>
+    <t>FISHERMAN</t>
+  </si>
+  <si>
+    <t>FLIGHT ATTENDANT</t>
+  </si>
+  <si>
+    <t>JEWELER</t>
+  </si>
+  <si>
+    <t>JUDGE</t>
+  </si>
+  <si>
+    <t>LAWYER</t>
+  </si>
+  <si>
+    <t>MECHANIC</t>
+  </si>
+  <si>
+    <t>MUSICIAN</t>
+  </si>
+  <si>
+    <t>NUTRITIONIST</t>
+  </si>
+  <si>
+    <t>NURSE</t>
+  </si>
+  <si>
+    <t>OPTICIAN</t>
+  </si>
+  <si>
+    <t>PAINTER</t>
+  </si>
+  <si>
+    <t>PHARMACIST</t>
+  </si>
+  <si>
+    <t>PHOTOGRAPHER</t>
+  </si>
+  <si>
+    <t>PHYSICIAN</t>
+  </si>
+  <si>
+    <t>PHYSICIAN'S ASSISTANT</t>
+  </si>
+  <si>
+    <t>PILOT</t>
+  </si>
+  <si>
+    <t>PLUMBER</t>
+  </si>
+  <si>
+    <t>POLICE OFFICER</t>
+  </si>
+  <si>
+    <t>POLITICIAN</t>
+  </si>
+  <si>
+    <t>PROFESSOR</t>
+  </si>
+  <si>
+    <t>PROGRAMMER</t>
+  </si>
+  <si>
+    <t>PSYCHOLOGIST</t>
+  </si>
+  <si>
+    <t>RECEPTIONIST</t>
+  </si>
+  <si>
+    <t>SALESMAN</t>
+  </si>
+  <si>
+    <t>SALESPERSON</t>
+  </si>
+  <si>
+    <t>SALESWOMAN</t>
+  </si>
+  <si>
+    <t>SECRETARY</t>
+  </si>
+  <si>
+    <t>SINGER</t>
+  </si>
+  <si>
+    <t>SURGEON</t>
+  </si>
+  <si>
+    <t>TEACHER</t>
+  </si>
+  <si>
+    <t>THERAPIST</t>
+  </si>
+  <si>
+    <t>TRANSLATOR</t>
+  </si>
+  <si>
+    <t>UNDERTAKER</t>
+  </si>
+  <si>
+    <t>VETERINARIAN</t>
+  </si>
+  <si>
+    <t>VIDEOGRAPHER</t>
+  </si>
+  <si>
+    <t>WAITER</t>
+  </si>
+  <si>
+    <t>WAITRESS</t>
+  </si>
+  <si>
+    <t>WRITER</t>
+  </si>
+  <si>
+    <t>DIPLOMAS</t>
+  </si>
+  <si>
+    <t>THREE YEAR BACHELOR PASS DEGREES</t>
+  </si>
+  <si>
+    <t>FOUR YEAR BACHELOR PASS DEGREES</t>
+  </si>
+  <si>
+    <t>FOUR YEAR BACHELOR HONOURS DEGREES</t>
+  </si>
+  <si>
+    <t>ONE YEAR BACHELOR HONOURS DEGREES</t>
+  </si>
+  <si>
+    <t>DOUBLE BACHELOR DEGREES</t>
+  </si>
+  <si>
+    <t>GRADUATE ENTRY BACHELOR DEGREES</t>
+  </si>
+  <si>
+    <t>GRADUATE CERTIFICATES</t>
+  </si>
+  <si>
+    <t>GRADUATE DIPLOMAS</t>
+  </si>
+  <si>
+    <t>MASTERS BY COURSEWORK DEGREES</t>
+  </si>
+  <si>
+    <t>MASTERS BY RESEARCH DEGREES</t>
+  </si>
+  <si>
+    <t>DOCTORAL DEGREES BY THESIS</t>
+  </si>
+  <si>
+    <t>HIGHER DOCTORAL DEGREES</t>
+  </si>
+  <si>
+    <t>HONORARY DOCTORAL DEGREES</t>
+  </si>
+  <si>
+    <t>Bachelor of Business</t>
+  </si>
+  <si>
+    <t>Bachelor of Commerce</t>
+  </si>
+  <si>
+    <t>Bachelor of Economics and Finance</t>
+  </si>
+  <si>
+    <t>Bachelor of Business Information Systems</t>
+  </si>
+  <si>
+    <t>Bachelor of Computer Science</t>
+  </si>
+  <si>
+    <t>Bachelor of Information Technology</t>
+  </si>
+  <si>
+    <t>Bachelor of Mathematics</t>
+  </si>
+  <si>
+    <t>Bachelor of Science (Physics)</t>
+  </si>
+  <si>
+    <t>Bachelor of Science (Materials)</t>
+  </si>
+  <si>
+    <t>Bachelor of Arts</t>
+  </si>
+  <si>
+    <t>Bachelor of Communication and Media</t>
+  </si>
+  <si>
+    <t>Bachelor of Creative Arts</t>
+  </si>
+  <si>
+    <t>Bachelor of Journalism</t>
+  </si>
+  <si>
+    <t>Bachelor of Performance</t>
+  </si>
+  <si>
+    <t>Bachelor of Politics, Philosophy and Economics</t>
+  </si>
+  <si>
+    <t>Bachelor of Health Science (Indigenous Health)</t>
+  </si>
+  <si>
+    <t>Bachelor of Marine Science</t>
+  </si>
+  <si>
+    <t>Bachelor of Medical and Health Sciences</t>
+  </si>
+  <si>
+    <t>Bachelor of Nursing</t>
+  </si>
+  <si>
+    <t>Bachelor of Nursing (Conversion)</t>
+  </si>
+  <si>
+    <t>Bachelor of Nursing (Overseas Qualified Nurses)</t>
+  </si>
+  <si>
+    <t>Bachelor of Nutrition Science</t>
+  </si>
+  <si>
+    <t>Bachelor of Pre-Medicine, Science and Health</t>
+  </si>
+  <si>
+    <t>Bachelor of Science</t>
+  </si>
+  <si>
+    <t>Bachelor of Exercise Science</t>
+  </si>
+  <si>
+    <t>Bachelor of Arts (Psychology)</t>
+  </si>
+  <si>
+    <t>Bachelor of Education Studies</t>
+  </si>
+  <si>
+    <t>Bachelor of Geography</t>
+  </si>
+  <si>
+    <t>Bachelor of Psychological Science</t>
+  </si>
+  <si>
+    <t>Bachelor of Public Health</t>
+  </si>
+  <si>
+    <t>Bachelor of Public Health (Dean’s Scholar)</t>
+  </si>
+  <si>
+    <t>Bachelor of Public Health Nutrition</t>
+  </si>
+  <si>
+    <t>Bachelor of Science (Psychology)</t>
+  </si>
+  <si>
+    <t>Bachelor of Social Science</t>
+  </si>
+  <si>
+    <t>Bachelor of Social Science (Dean’s Scholar)</t>
+  </si>
+  <si>
+    <t>Bachelor of Social Science (Psychology)</t>
+  </si>
+  <si>
+    <t>Bachelor of Sustainable Communities</t>
+  </si>
+  <si>
+    <t>Bachelor of Laws (Direct Entry)</t>
+  </si>
+  <si>
+    <t>Bachelor of Education - The Early Years</t>
+  </si>
+  <si>
+    <t>Bachelor of Education - The Early Years (Dean’s Scholar)</t>
+  </si>
+  <si>
+    <t>Bachelor of Health and Physical Education</t>
+  </si>
+  <si>
+    <t>Bachelor of Health and Physical Education (Dean’s Scholar)</t>
+  </si>
+  <si>
+    <t>Bachelor of Mathematics Education</t>
+  </si>
+  <si>
+    <t>Bachelor of Mathematics Education (Dean’s Scholar)</t>
+  </si>
+  <si>
+    <t>Bachelor of Primary Education</t>
+  </si>
+  <si>
+    <t>Bachelor of Primary Education (Dean’s Scholar)</t>
+  </si>
+  <si>
+    <t>Bachelor of Science Education</t>
+  </si>
+  <si>
+    <t>Bachelor of Science Education (Dean's Scholar)</t>
+  </si>
+  <si>
+    <t>Bachelor of Social Work</t>
+  </si>
+  <si>
+    <t>Master of Autism </t>
+  </si>
+  <si>
+    <t>MAut</t>
+  </si>
+  <si>
+    <t>Master of Education </t>
+  </si>
+  <si>
+    <t>MEd</t>
+  </si>
+  <si>
+    <t>Master of Education Advanced </t>
+  </si>
+  <si>
+    <t>MEdAdv</t>
+  </si>
+  <si>
+    <t>Master of Educational Studies </t>
+  </si>
+  <si>
+    <t>MEdSt</t>
+  </si>
+  <si>
+    <t>Master of Physical and Health Education </t>
+  </si>
+  <si>
+    <t>MPhyHlthEd</t>
+  </si>
+  <si>
+    <t>Master of Professional Psychology </t>
+  </si>
+  <si>
+    <t>MProfPsyc</t>
+  </si>
+  <si>
+    <t>Master of Psychology (Clinical) </t>
+  </si>
+  <si>
+    <t>MPsyc(Clin)</t>
+  </si>
+  <si>
+    <t>Master of Public Health </t>
+  </si>
+  <si>
+    <t>MPubHlth</t>
+  </si>
+  <si>
+    <t>Master of Public Health Advanced </t>
+  </si>
+  <si>
+    <t>MPubHlthAdv</t>
+  </si>
+  <si>
+    <t>Master of Social Work (Qualifying)</t>
+  </si>
+  <si>
+    <t>MSocWork(Qual)</t>
+  </si>
+  <si>
+    <t>Master of Special Education </t>
+  </si>
+  <si>
+    <t>MSpecEd</t>
+  </si>
+  <si>
+    <t>Master of Teaching (Primary) </t>
+  </si>
+  <si>
+    <t>MTeach(Prim)</t>
+  </si>
+  <si>
+    <t>Master of Teaching (Secondary) </t>
+  </si>
+  <si>
+    <t>MTeach(Sec)</t>
+  </si>
+  <si>
+    <t>Master of Work Health and Safety </t>
+  </si>
+  <si>
+    <t>MWHS</t>
+  </si>
+  <si>
+    <t>Master of Work Health and Safety Advanced </t>
+  </si>
+  <si>
+    <t>Doctor of Medicine</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>International Master of Science </t>
+  </si>
+  <si>
+    <t>IntMSc</t>
+  </si>
+  <si>
+    <t>Master of Clinical Exercise Physiology </t>
+  </si>
+  <si>
+    <t>MClinExPhysi</t>
+  </si>
+  <si>
+    <t>Master of Health Leadership and Management </t>
+  </si>
+  <si>
+    <t>MHLM</t>
+  </si>
+  <si>
+    <t>Master of Indigenous Health </t>
+  </si>
+  <si>
+    <t>MIndHlth</t>
+  </si>
+  <si>
+    <t>Master of Nursing </t>
+  </si>
+  <si>
+    <t>MNurse</t>
+  </si>
+  <si>
+    <t>Master of Nursing (Mental Health) </t>
+  </si>
+  <si>
+    <t>MNurse(MntlHlth)</t>
+  </si>
+  <si>
+    <t>Master of Nursing International </t>
+  </si>
+  <si>
+    <t>MNursInt</t>
+  </si>
+  <si>
+    <t>Master of Nutrition and Dietetics</t>
+  </si>
+  <si>
+    <t>MNutr&amp;Diet</t>
+  </si>
+  <si>
+    <t>Master of Science </t>
+  </si>
+  <si>
+    <t>MSc</t>
+  </si>
+  <si>
+    <t>Master of Science and Management </t>
+  </si>
+  <si>
+    <t>MScMgmt</t>
+  </si>
+  <si>
+    <t>Master of Science (Dementia Care) </t>
+  </si>
+  <si>
+    <t>MSc(DementiaCare)</t>
+  </si>
+  <si>
+    <t>Master of Science (Gerontology and Rehabilitation Studies) </t>
+  </si>
+  <si>
+    <t>Master of Fisheries Policy </t>
+  </si>
+  <si>
+    <t>MFishPol</t>
+  </si>
+  <si>
+    <t>Master of International Studies </t>
+  </si>
+  <si>
+    <t>MIntlSt</t>
+  </si>
+  <si>
+    <t>Master of International Studies Advanced </t>
+  </si>
+  <si>
+    <t>MIntStAdv</t>
+  </si>
+  <si>
+    <t>Master of Laws (Criminal Practice) </t>
+  </si>
+  <si>
+    <t>LLM(CrimPrac)</t>
+  </si>
+  <si>
+    <t>Master of Maritime Policy </t>
+  </si>
+  <si>
+    <t>MMaritimePol</t>
+  </si>
+  <si>
+    <t>Master of Maritime Studies </t>
+  </si>
+  <si>
+    <t>Master of Applied Finance </t>
+  </si>
+  <si>
+    <t> MAppFin</t>
+  </si>
+  <si>
+    <t>Master of Business </t>
+  </si>
+  <si>
+    <t> MBus</t>
+  </si>
+  <si>
+    <t>Master of Business Administration </t>
+  </si>
+  <si>
+    <t> MBA</t>
+  </si>
+  <si>
+    <t>Master of Business Administration (Executive) </t>
+  </si>
+  <si>
+    <t> EMBA </t>
+  </si>
+  <si>
+    <t>Master of Business Administration Advanced </t>
+  </si>
+  <si>
+    <t> MBAAdv</t>
+  </si>
+  <si>
+    <t>Master of Business Coaching </t>
+  </si>
+  <si>
+    <t> MBusCoach</t>
+  </si>
+  <si>
+    <t>Master of Professional Accounting </t>
+  </si>
+  <si>
+    <t> MProfAccy</t>
+  </si>
+  <si>
+    <t>Master of Professional Accounting Advanced </t>
+  </si>
+  <si>
+    <t> MProfAccyAdv</t>
+  </si>
+  <si>
+    <t>MCompSc</t>
+  </si>
+  <si>
+    <t>Master of Electrical Power Engineering </t>
+  </si>
+  <si>
+    <t>MElecPowEng</t>
+  </si>
+  <si>
+    <t>Master of Engineering </t>
+  </si>
+  <si>
+    <t>MEng</t>
+  </si>
+  <si>
+    <t>Master of Engineering (Electrical Traction Networks) </t>
+  </si>
+  <si>
+    <t>MEng(ElecTracNet)</t>
+  </si>
+  <si>
+    <t>Master of Engineering Asset Management </t>
+  </si>
+  <si>
+    <t>MEngAssetMgmt</t>
+  </si>
+  <si>
+    <t>Master of Engineering Management </t>
+  </si>
+  <si>
+    <t>MEngMgmt</t>
+  </si>
+  <si>
+    <t>Master of Engineering Science </t>
+  </si>
+  <si>
+    <t>MEngSc</t>
+  </si>
+  <si>
+    <t>Master of Financial Mathematics </t>
+  </si>
+  <si>
+    <t>MFinMath</t>
+  </si>
+  <si>
+    <t>Master of Health Informatics </t>
+  </si>
+  <si>
+    <t>MHlthInfo</t>
+  </si>
+  <si>
+    <t>Master of Information and Communication Technology Advanced </t>
+  </si>
+  <si>
+    <t>MICTAdv</t>
+  </si>
+  <si>
+    <t>Master of Information Technology </t>
+  </si>
+  <si>
+    <t>MIT</t>
+  </si>
+  <si>
+    <t>Master of Information Technology Management </t>
+  </si>
+  <si>
+    <t>MITMgmt</t>
+  </si>
+  <si>
+    <t>Master of Information Technology Studies Advanced </t>
+  </si>
+  <si>
+    <t>MITStAdv</t>
+  </si>
+  <si>
+    <t>Master of Mathematics </t>
+  </si>
+  <si>
+    <t>MMath</t>
+  </si>
+  <si>
+    <t>Master of Medical Radiation Physics </t>
+  </si>
+  <si>
+    <t>MMedRadPhys</t>
+  </si>
+  <si>
+    <t>Master of Rolling Stock Engineering </t>
+  </si>
+  <si>
+    <t>MRollStockEng</t>
+  </si>
+  <si>
+    <t>Master of Science (Medical Radiation Physics) </t>
+  </si>
+  <si>
+    <t>MSc(MedRadPhys)</t>
+  </si>
+  <si>
+    <t>Master of Statistics </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7265,8 +8011,22 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7279,8 +8039,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -7303,11 +8069,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFEEEEEE"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFEEEEEE"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFEEEEEE"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFEEEEEE"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFEEEEEE"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFEEEEEE"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFEEEEEE"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFEEEEEE"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFEEEEEE"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFEEEEEE"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFEEEEEE"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFEEEEEE"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -7324,8 +8188,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9559,7 +10445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1064"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1019" workbookViewId="0">
+    <sheetView topLeftCell="A1019" workbookViewId="0">
       <selection activeCell="J1030" sqref="J1030"/>
     </sheetView>
   </sheetViews>
@@ -34039,4 +34925,1311 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:B71"/>
+  <sheetViews>
+    <sheetView topLeftCell="A40" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>2334</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2336</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2337</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2338</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>2339</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>2340</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>2341</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>2342</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>2343</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>2344</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>2346</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>2348</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>2349</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>2351</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>2352</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>2353</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>2354</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>2355</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>2356</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>2357</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>2359</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>2360</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>2361</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>2362</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>2363</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>2364</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>2365</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>2366</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>2368</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>2369</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>2370</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>2371</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>2372</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>2373</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>2374</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>2376</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>2377</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>2378</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>2379</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>2381</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>2382</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>2383</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>2384</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>2385</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>2386</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>2387</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>2388</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>2389</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>2390</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>2391</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>2395</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>2396</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>2397</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>2397</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>2398</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>2399</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>2402</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>2403</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D111"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94:D111"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>2404</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2418</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>2405</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2419</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2406</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2407</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>2421</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2408</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>2409</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>2410</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>2424</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>2411</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>2412</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>2413</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>2427</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>2414</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>2415</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>2429</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>2416</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>2430</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>2417</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>2431</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="8" t="s">
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="8" t="s">
+        <v>2442</v>
+      </c>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="11" t="s">
+        <v>2433</v>
+      </c>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="11" t="s">
+        <v>2434</v>
+      </c>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="11" t="s">
+        <v>2435</v>
+      </c>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="11" t="s">
+        <v>2436</v>
+      </c>
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="11" t="s">
+        <v>2437</v>
+      </c>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="11" t="s">
+        <v>2438</v>
+      </c>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="11" t="s">
+        <v>2439</v>
+      </c>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="11" t="s">
+        <v>2440</v>
+      </c>
+      <c r="D24" s="12"/>
+    </row>
+    <row r="25" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="13" t="s">
+        <v>2441</v>
+      </c>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="15" t="s">
+        <v>2443</v>
+      </c>
+      <c r="D26" s="16"/>
+    </row>
+    <row r="27" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="11" t="s">
+        <v>2444</v>
+      </c>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="11" t="s">
+        <v>2445</v>
+      </c>
+      <c r="D28" s="12"/>
+    </row>
+    <row r="29" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="11" t="s">
+        <v>2446</v>
+      </c>
+      <c r="D29" s="12"/>
+    </row>
+    <row r="30" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="11" t="s">
+        <v>2447</v>
+      </c>
+      <c r="D30" s="12"/>
+    </row>
+    <row r="31" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="11" t="s">
+        <v>2448</v>
+      </c>
+      <c r="D31" s="12"/>
+    </row>
+    <row r="32" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="11" t="s">
+        <v>2449</v>
+      </c>
+      <c r="D32" s="12"/>
+    </row>
+    <row r="33" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="11" t="s">
+        <v>2450</v>
+      </c>
+      <c r="D33" s="12"/>
+    </row>
+    <row r="34" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="11" t="s">
+        <v>2441</v>
+      </c>
+      <c r="D34" s="12"/>
+    </row>
+    <row r="35" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="11" t="s">
+        <v>2451</v>
+      </c>
+      <c r="D35" s="12"/>
+    </row>
+    <row r="36" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="11" t="s">
+        <v>2452</v>
+      </c>
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="11" t="s">
+        <v>2453</v>
+      </c>
+      <c r="D37" s="12"/>
+    </row>
+    <row r="38" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="13" t="s">
+        <v>2454</v>
+      </c>
+      <c r="D38" s="14"/>
+    </row>
+    <row r="39" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="8" t="s">
+        <v>2455</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="15" t="s">
+        <v>2456</v>
+      </c>
+      <c r="D40" s="16"/>
+    </row>
+    <row r="41" spans="3:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="11" t="s">
+        <v>2457</v>
+      </c>
+      <c r="D41" s="12"/>
+    </row>
+    <row r="42" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="11" t="s">
+        <v>2458</v>
+      </c>
+      <c r="D42" s="12"/>
+    </row>
+    <row r="43" spans="3:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="11" t="s">
+        <v>2459</v>
+      </c>
+      <c r="D43" s="12"/>
+    </row>
+    <row r="44" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="11" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D44" s="12"/>
+    </row>
+    <row r="45" spans="3:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="11" t="s">
+        <v>2461</v>
+      </c>
+      <c r="D45" s="12"/>
+    </row>
+    <row r="46" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="11" t="s">
+        <v>2462</v>
+      </c>
+      <c r="D46" s="12"/>
+    </row>
+    <row r="47" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="11" t="s">
+        <v>2463</v>
+      </c>
+      <c r="D47" s="12"/>
+    </row>
+    <row r="48" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="11" t="s">
+        <v>2464</v>
+      </c>
+      <c r="D48" s="12"/>
+    </row>
+    <row r="49" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="11" t="s">
+        <v>2465</v>
+      </c>
+      <c r="D49" s="12"/>
+    </row>
+    <row r="50" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="13" t="s">
+        <v>2466</v>
+      </c>
+      <c r="D50" s="14"/>
+    </row>
+    <row r="51" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="15" t="s">
+        <v>2467</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>2468</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="11" t="s">
+        <v>2469</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>2470</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="11" t="s">
+        <v>2471</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>2472</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="11" t="s">
+        <v>2473</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>2474</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="11" t="s">
+        <v>2475</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="11" t="s">
+        <v>2477</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="11" t="s">
+        <v>2479</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="11" t="s">
+        <v>2481</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>2482</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="11" t="s">
+        <v>2483</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>2484</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="11" t="s">
+        <v>2485</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>2486</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="11" t="s">
+        <v>2487</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>2488</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="11" t="s">
+        <v>2489</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>2490</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C63" s="11" t="s">
+        <v>2491</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>2492</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="11" t="s">
+        <v>2493</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>2494</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C65" s="13" t="s">
+        <v>2495</v>
+      </c>
+      <c r="D65" s="14"/>
+    </row>
+    <row r="66" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="15" t="s">
+        <v>2496</v>
+      </c>
+      <c r="D66" s="16" t="s">
+        <v>2497</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="11" t="s">
+        <v>2498</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>2499</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C68" s="11" t="s">
+        <v>2500</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C69" s="11" t="s">
+        <v>2502</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>2503</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="11" t="s">
+        <v>2504</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>2505</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="11" t="s">
+        <v>2506</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>2507</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C72" s="11" t="s">
+        <v>2508</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>2509</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C73" s="11" t="s">
+        <v>2510</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C74" s="11" t="s">
+        <v>2512</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>2513</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C75" s="11" t="s">
+        <v>2514</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>2515</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="11" t="s">
+        <v>2516</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>2517</v>
+      </c>
+    </row>
+    <row r="77" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="11" t="s">
+        <v>2518</v>
+      </c>
+      <c r="D77" s="12" t="s">
+        <v>2519</v>
+      </c>
+    </row>
+    <row r="78" spans="3:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C78" s="13" t="s">
+        <v>2520</v>
+      </c>
+      <c r="D78" s="14"/>
+    </row>
+    <row r="79" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C79" s="15" t="s">
+        <v>2521</v>
+      </c>
+      <c r="D79" s="16" t="s">
+        <v>2522</v>
+      </c>
+    </row>
+    <row r="80" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C80" s="11" t="s">
+        <v>2523</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>2524</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C81" s="11" t="s">
+        <v>2525</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>2526</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C82" s="11" t="s">
+        <v>2527</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>2528</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C83" s="11" t="s">
+        <v>2529</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>2530</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C84" s="13" t="s">
+        <v>2531</v>
+      </c>
+      <c r="D84" s="14"/>
+    </row>
+    <row r="85" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C85" s="15" t="s">
+        <v>2532</v>
+      </c>
+      <c r="D85" s="16" t="s">
+        <v>2533</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C86" s="11" t="s">
+        <v>2534</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>2535</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C87" s="11" t="s">
+        <v>2536</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>2537</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C88" s="11" t="s">
+        <v>2538</v>
+      </c>
+      <c r="D88" s="12" t="s">
+        <v>2539</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C89" s="11" t="s">
+        <v>2540</v>
+      </c>
+      <c r="D89" s="12" t="s">
+        <v>2541</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C90" s="11" t="s">
+        <v>2542</v>
+      </c>
+      <c r="D90" s="12" t="s">
+        <v>2543</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C91" s="11" t="s">
+        <v>2544</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>2545</v>
+      </c>
+    </row>
+    <row r="92" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C92" s="11" t="s">
+        <v>2546</v>
+      </c>
+      <c r="D92" s="12" t="s">
+        <v>2547</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C93" s="13" t="s">
+        <v>2514</v>
+      </c>
+      <c r="D93" s="14"/>
+    </row>
+    <row r="94" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C94" s="9" t="s">
+        <v>2548</v>
+      </c>
+      <c r="D94" s="10"/>
+    </row>
+    <row r="95" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C95" s="11" t="s">
+        <v>2549</v>
+      </c>
+      <c r="D95" s="12" t="s">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C96" s="11" t="s">
+        <v>2551</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>2552</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C97" s="11" t="s">
+        <v>2553</v>
+      </c>
+      <c r="D97" s="12" t="s">
+        <v>2554</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C98" s="11" t="s">
+        <v>2555</v>
+      </c>
+      <c r="D98" s="12" t="s">
+        <v>2556</v>
+      </c>
+    </row>
+    <row r="99" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C99" s="11" t="s">
+        <v>2557</v>
+      </c>
+      <c r="D99" s="12" t="s">
+        <v>2558</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C100" s="11" t="s">
+        <v>2559</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="101" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C101" s="11" t="s">
+        <v>2561</v>
+      </c>
+      <c r="D101" s="12" t="s">
+        <v>2562</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C102" s="11" t="s">
+        <v>2563</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>2564</v>
+      </c>
+    </row>
+    <row r="103" spans="3:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C103" s="11" t="s">
+        <v>2565</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="104" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C104" s="11" t="s">
+        <v>2567</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>2568</v>
+      </c>
+    </row>
+    <row r="105" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C105" s="11" t="s">
+        <v>2569</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>2570</v>
+      </c>
+    </row>
+    <row r="106" spans="3:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C106" s="11" t="s">
+        <v>2571</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>2572</v>
+      </c>
+    </row>
+    <row r="107" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C107" s="11" t="s">
+        <v>2573</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>2574</v>
+      </c>
+    </row>
+    <row r="108" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C108" s="11" t="s">
+        <v>2575</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>2576</v>
+      </c>
+    </row>
+    <row r="109" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C109" s="11" t="s">
+        <v>2577</v>
+      </c>
+      <c r="D109" s="12" t="s">
+        <v>2578</v>
+      </c>
+    </row>
+    <row r="110" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C110" s="11" t="s">
+        <v>2579</v>
+      </c>
+      <c r="D110" s="12" t="s">
+        <v>2580</v>
+      </c>
+    </row>
+    <row r="111" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C111" s="13" t="s">
+        <v>2581</v>
+      </c>
+      <c r="D111" s="14"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000086"/>
+    <hyperlink ref="C2" r:id="rId2" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006744"/>
+    <hyperlink ref="C3" r:id="rId3" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000087"/>
+    <hyperlink ref="C4" r:id="rId4" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18008064"/>
+    <hyperlink ref="C5" r:id="rId5" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18009041"/>
+    <hyperlink ref="C6" r:id="rId6" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18009042"/>
+    <hyperlink ref="C7" r:id="rId7" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006876"/>
+    <hyperlink ref="C8" r:id="rId8" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000102"/>
+    <hyperlink ref="C9" r:id="rId9" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006080"/>
+    <hyperlink ref="C10" r:id="rId10" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18005888"/>
+    <hyperlink ref="C11" r:id="rId11" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18005922"/>
+    <hyperlink ref="C12" r:id="rId12" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000056"/>
+    <hyperlink ref="C13" r:id="rId13" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006046"/>
+    <hyperlink ref="C14" r:id="rId14" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006037"/>
+    <hyperlink ref="C15" r:id="rId15" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000197"/>
+    <hyperlink ref="C17" r:id="rId16" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006095"/>
+    <hyperlink ref="C18" r:id="rId17" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000205"/>
+    <hyperlink ref="C19" r:id="rId18" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000051"/>
+    <hyperlink ref="C20" r:id="rId19" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006100"/>
+    <hyperlink ref="C21" r:id="rId20" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006101"/>
+    <hyperlink ref="C22" r:id="rId21" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000059"/>
+    <hyperlink ref="C23" r:id="rId22" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006108"/>
+    <hyperlink ref="C24" r:id="rId23" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18008078"/>
+    <hyperlink ref="C25" r:id="rId24" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006141"/>
+    <hyperlink ref="C16" r:id="rId25" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006106"/>
+    <hyperlink ref="C26" r:id="rId26" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006093"/>
+    <hyperlink ref="C27" r:id="rId27" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18066571"/>
+    <hyperlink ref="C28" r:id="rId28" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18009022"/>
+    <hyperlink ref="C29" r:id="rId29" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18008083"/>
+    <hyperlink ref="C30" r:id="rId30" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000054"/>
+    <hyperlink ref="C31" r:id="rId31" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18008086"/>
+    <hyperlink ref="C32" r:id="rId32" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000055"/>
+    <hyperlink ref="C33" r:id="rId33" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000170"/>
+    <hyperlink ref="C34" r:id="rId34" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000211"/>
+    <hyperlink ref="C35" r:id="rId35" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000208"/>
+    <hyperlink ref="C36" r:id="rId36" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000267"/>
+    <hyperlink ref="C37" r:id="rId37" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000207"/>
+    <hyperlink ref="C38" r:id="rId38" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18066569"/>
+    <hyperlink ref="C39" r:id="rId39" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006126"/>
+    <hyperlink ref="C40" r:id="rId40" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006055"/>
+    <hyperlink ref="C41" r:id="rId41" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000045"/>
+    <hyperlink ref="C42" r:id="rId42" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18008058"/>
+    <hyperlink ref="C43" r:id="rId43" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000047"/>
+    <hyperlink ref="C44" r:id="rId44" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006065"/>
+    <hyperlink ref="C45" r:id="rId45" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000046"/>
+    <hyperlink ref="C46" r:id="rId46" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006059"/>
+    <hyperlink ref="C47" r:id="rId47" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000048"/>
+    <hyperlink ref="C48" r:id="rId48" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006066"/>
+    <hyperlink ref="C49" r:id="rId49" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000049"/>
+    <hyperlink ref="C50" r:id="rId50" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000268"/>
+    <hyperlink ref="C51" r:id="rId51" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18066573"/>
+    <hyperlink ref="C52" r:id="rId52" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006185"/>
+    <hyperlink ref="C53" r:id="rId53" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18009007"/>
+    <hyperlink ref="C54" r:id="rId54" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000275"/>
+    <hyperlink ref="C55" r:id="rId55" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006186"/>
+    <hyperlink ref="C56" r:id="rId56" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000220"/>
+    <hyperlink ref="C57" r:id="rId57" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006804"/>
+    <hyperlink ref="C58" r:id="rId58" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006784"/>
+    <hyperlink ref="C59" r:id="rId59" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000085"/>
+    <hyperlink ref="C60" r:id="rId60" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18066572"/>
+    <hyperlink ref="C61" r:id="rId61" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000271"/>
+    <hyperlink ref="C62" r:id="rId62" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000215"/>
+    <hyperlink ref="C63" r:id="rId63" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000216"/>
+    <hyperlink ref="C64" r:id="rId64" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000217"/>
+    <hyperlink ref="C65" r:id="rId65" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18008087"/>
+    <hyperlink ref="C66" r:id="rId66" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18009009"/>
+    <hyperlink ref="C67" r:id="rId67" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000202"/>
+    <hyperlink ref="C68" r:id="rId68" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006774"/>
+    <hyperlink ref="C69" r:id="rId69" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006783"/>
+    <hyperlink ref="C70" r:id="rId70" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006789"/>
+    <hyperlink ref="C71" r:id="rId71" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006790"/>
+    <hyperlink ref="C72" r:id="rId72" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006791"/>
+    <hyperlink ref="C73" r:id="rId73" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18009008"/>
+    <hyperlink ref="C74" r:id="rId74" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006776"/>
+    <hyperlink ref="C75" r:id="rId75" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18048459"/>
+    <hyperlink ref="C76" r:id="rId76" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000067"/>
+    <hyperlink ref="C77" r:id="rId77" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000014"/>
+    <hyperlink ref="C78" r:id="rId78" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006793"/>
+    <hyperlink ref="C79" r:id="rId79" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000066"/>
+    <hyperlink ref="C80" r:id="rId80" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18005952"/>
+    <hyperlink ref="C81" r:id="rId81" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18008077"/>
+    <hyperlink ref="C82" r:id="rId82" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000032"/>
+    <hyperlink ref="C83" r:id="rId83" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006934"/>
+    <hyperlink ref="C84" r:id="rId84" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18007233"/>
+    <hyperlink ref="C85" r:id="rId85" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006000"/>
+    <hyperlink ref="C86" r:id="rId86" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000192"/>
+    <hyperlink ref="C87" r:id="rId87" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18008040"/>
+    <hyperlink ref="C88" r:id="rId88" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000140"/>
+    <hyperlink ref="C89" r:id="rId89" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18008041"/>
+    <hyperlink ref="C90" r:id="rId90" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18008061"/>
+    <hyperlink ref="C91" r:id="rId91" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18008073"/>
+    <hyperlink ref="C92" r:id="rId92" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18008073"/>
+    <hyperlink ref="C93" r:id="rId93" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18008045"/>
+    <hyperlink ref="C95" r:id="rId94" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000097"/>
+    <hyperlink ref="C96" r:id="rId95" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000095"/>
+    <hyperlink ref="C97" r:id="rId96" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000172"/>
+    <hyperlink ref="C98" r:id="rId97" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006216"/>
+    <hyperlink ref="C99" r:id="rId98" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006215"/>
+    <hyperlink ref="C100" r:id="rId99" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18066567"/>
+    <hyperlink ref="C101" r:id="rId100" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18007208"/>
+    <hyperlink ref="C102" r:id="rId101" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18007209"/>
+    <hyperlink ref="C103" r:id="rId102" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18007213"/>
+    <hyperlink ref="C104" r:id="rId103" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000196"/>
+    <hyperlink ref="C105" r:id="rId104" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18007215"/>
+    <hyperlink ref="C106" r:id="rId105" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18005982"/>
+    <hyperlink ref="C107" r:id="rId106" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18007217"/>
+    <hyperlink ref="C108" r:id="rId107" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18006217"/>
+    <hyperlink ref="C109" r:id="rId108" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18008059"/>
+    <hyperlink ref="C110" r:id="rId109" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18000031"/>
+    <hyperlink ref="C111" r:id="rId110" display="https://documents.uow.edu.au/handbook/yr2018/ug/ssLINK/H18007220"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>